<commit_message>
Update Template2.xlsx with content modifications
Modified the binary structure of Template2.xlsx. Specific changes are not detailed, but the file has been altered in terms of content or structure.
</commit_message>
<xml_diff>
--- a/Demo/Template2.xlsx
+++ b/Demo/Template2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erekl\source\repos\NCER-QuTIe\DemoProject\Demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5648294-5F03-4F14-867C-9B7C6F410C4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773623EE-EB94-46CD-B788-2379A302FC18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -76,20 +76,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="hh\:mm\:ss"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -207,23 +197,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -238,7 +226,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -521,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B49A9BA3-4985-4643-B189-3DC59E2B94A3}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -540,57 +528,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="10"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A3" s="11"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
     </row>
-    <row r="6" spans="1:9" s="4" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:9" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -602,11 +590,6 @@
     <row r="12" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="13" spans="1:9" ht="21.45" customHeight="1" x14ac:dyDescent="0.4"/>
     <row r="14" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>